<commit_message>
Unit testing made easy. Darn easy.
</commit_message>
<xml_diff>
--- a/testing/samples/UIData.xlsx
+++ b/testing/samples/UIData.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>textValue</t>
   </si>
@@ -37,6 +38,18 @@
   </si>
   <si>
     <t>Nice thing!</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
   </si>
 </sst>
 </file>
@@ -407,7 +420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -448,4 +461,48 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
now this is a good demo. Lacking features  :  method level run.
</commit_message>
<xml_diff>
--- a/testing/samples/UIData.xlsx
+++ b/testing/samples/UIData.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="add" sheetId="2" r:id="rId2"/>
+    <sheet name="sub" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>textValue</t>
   </si>
@@ -46,20 +47,39 @@
     <t>b</t>
   </si>
   <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>A2</t>
+    <t>op</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -82,13 +102,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -465,36 +489,99 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="C1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="C2" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3">
         <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding globals support to the NAPI.
</commit_message>
<xml_diff>
--- a/testing/samples/UIData.xlsx
+++ b/testing/samples/UIData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>textValue</t>
   </si>
@@ -45,15 +45,6 @@
   </si>
   <si>
     <t>b</t>
-  </si>
-  <si>
-    <t>op</t>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
 </sst>
 </file>
@@ -489,45 +480,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -543,45 +525,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>10</v>
       </c>
       <c r="B2">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>12</v>
       </c>
       <c r="B3">
         <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding excel formula support!
</commit_message>
<xml_diff>
--- a/testing/samples/UIData.xlsx
+++ b/testing/samples/UIData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="add" sheetId="2" r:id="rId2"/>
     <sheet name="sub" sheetId="3" r:id="rId3"/>
+    <sheet name="Formula" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -482,7 +483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
@@ -565,4 +566,51 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <f>A1*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="B2:B3" si="0">A2*10</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixing the web suite, making sure rest call happens. Tried and tested.
</commit_message>
<xml_diff>
--- a/testing/samples/UIData.xlsx
+++ b/testing/samples/UIData.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="add" sheetId="2" r:id="rId2"/>
     <sheet name="sub" sheetId="3" r:id="rId3"/>
     <sheet name="Formula" sheetId="4" r:id="rId4"/>
+    <sheet name="APIData" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>textValue</t>
   </si>
@@ -46,6 +47,15 @@
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>symbol</t>
+  </si>
+  <si>
+    <t>INFY</t>
+  </si>
+  <si>
+    <t>ADSL</t>
   </si>
 </sst>
 </file>
@@ -572,7 +582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B3"/>
     </sheetView>
   </sheetViews>
@@ -603,6 +613,41 @@
       <c r="B3">
         <f t="shared" si="0"/>
         <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding the feature : base , and method is now there in both web app and feature level. Caller gets generated per feature.
</commit_message>
<xml_diff>
--- a/testing/samples/UIData.xlsx
+++ b/testing/samples/UIData.xlsx
@@ -11,7 +11,7 @@
     <sheet name="add" sheetId="2" r:id="rId2"/>
     <sheet name="sub" sheetId="3" r:id="rId3"/>
     <sheet name="Formula" sheetId="4" r:id="rId4"/>
-    <sheet name="APIData" sheetId="5" r:id="rId5"/>
+    <sheet name="userId" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>textValue</t>
   </si>
@@ -49,13 +49,7 @@
     <t>b</t>
   </si>
   <si>
-    <t>symbol</t>
-  </si>
-  <si>
-    <t>INFY</t>
-  </si>
-  <si>
-    <t>ADSL</t>
+    <t>userId</t>
   </si>
 </sst>
 </file>
@@ -629,9 +623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
@@ -641,13 +633,13 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>9</v>
+      <c r="A2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>10</v>
+      <c r="A3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing ignore, and adding assertion support.
</commit_message>
<xml_diff>
--- a/testing/samples/UIData.xlsx
+++ b/testing/samples/UIData.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>textValue</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>userId</t>
+  </si>
+  <si>
+    <t>#enable#</t>
   </si>
 </sst>
 </file>
@@ -621,25 +624,52 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding randomization of test run, tested.
</commit_message>
<xml_diff>
--- a/testing/samples/UIData.xlsx
+++ b/testing/samples/UIData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -535,7 +535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -664,10 +664,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -710,6 +710,30 @@
       </c>
       <c r="B5" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>